<commit_message>
partial opus-big lsp simple adapt wce results
</commit_message>
<xml_diff>
--- a/model_evaluations/Opus-Big Hyperparameter Search Results.xlsx
+++ b/model_evaluations/Opus-Big Hyperparameter Search Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ers19_ic_ac_uk/Documents/MSc Computing/Individual Project/Code/medical-mt/model_evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2634" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9F6A047-246D-4A60-B272-06D36BFB10F3}"/>
+  <xr:revisionPtr revIDLastSave="2667" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E0BE7FF-19AA-4940-B43F-60631739CA36}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_big Validation" sheetId="7" r:id="rId1"/>
@@ -520,30 +520,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -574,6 +550,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -582,6 +564,27 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -593,9 +596,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -927,13 +927,13 @@
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="33">
+      <c r="C2" s="48">
         <v>0.25</v>
       </c>
       <c r="D2" s="4">
@@ -955,9 +955,9 @@
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="31"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
       <c r="D3" s="6">
         <v>1.5</v>
       </c>
@@ -977,9 +977,9 @@
       <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="31"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
       <c r="D4" s="6">
         <v>1.75</v>
       </c>
@@ -999,9 +999,9 @@
       <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="31"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
       <c r="D5" s="6">
         <v>2</v>
       </c>
@@ -1021,9 +1021,9 @@
       <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="31"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34">
+      <c r="A6" s="46"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40">
         <v>0.5</v>
       </c>
       <c r="D6" s="6">
@@ -1045,9 +1045,9 @@
       <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="31"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
+      <c r="A7" s="46"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="6">
         <v>1.5</v>
       </c>
@@ -1067,9 +1067,9 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="31"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
       <c r="D8" s="6">
         <v>1.75</v>
       </c>
@@ -1089,9 +1089,9 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="31"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
+      <c r="A9" s="46"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
       <c r="D9" s="6">
         <v>2</v>
       </c>
@@ -1111,9 +1111,9 @@
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="31"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34">
+      <c r="A10" s="46"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40">
         <v>0.75</v>
       </c>
       <c r="D10" s="6">
@@ -1135,9 +1135,9 @@
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="31"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
+      <c r="A11" s="46"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
       <c r="D11" s="6">
         <v>1.5</v>
       </c>
@@ -1157,9 +1157,9 @@
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="31"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
+      <c r="A12" s="46"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
       <c r="D12" s="6">
         <v>1.75</v>
       </c>
@@ -1179,9 +1179,9 @@
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="31"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
+      <c r="A13" s="46"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
       <c r="D13" s="6">
         <v>2</v>
       </c>
@@ -1201,9 +1201,9 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="31"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34">
+      <c r="A14" s="46"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40">
         <v>1</v>
       </c>
       <c r="D14" s="6">
@@ -1225,9 +1225,9 @@
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="31"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
+      <c r="A15" s="46"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
       <c r="D15" s="6">
         <v>1.5</v>
       </c>
@@ -1247,9 +1247,9 @@
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="31"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
+      <c r="A16" s="46"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
       <c r="D16" s="6">
         <v>1.75</v>
       </c>
@@ -1269,9 +1269,9 @@
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="31"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
       <c r="D17" s="6">
         <v>2</v>
       </c>
@@ -1291,11 +1291,11 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="31"/>
-      <c r="B18" s="36">
+      <c r="A18" s="46"/>
+      <c r="B18" s="49">
         <v>1</v>
       </c>
-      <c r="C18" s="34"/>
+      <c r="C18" s="40"/>
       <c r="D18" s="6">
         <v>1.25</v>
       </c>
@@ -1315,9 +1315,9 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="31"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="34"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="40"/>
       <c r="D19" s="6">
         <v>1.5</v>
       </c>
@@ -1337,9 +1337,9 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="31"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="34"/>
+      <c r="A20" s="46"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="40"/>
       <c r="D20" s="6">
         <v>1.75</v>
       </c>
@@ -1359,9 +1359,9 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="31"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="34"/>
+      <c r="A21" s="46"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
@@ -1381,11 +1381,11 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="31"/>
-      <c r="B22" s="34">
+      <c r="A22" s="46"/>
+      <c r="B22" s="40">
         <v>0.75</v>
       </c>
-      <c r="C22" s="34"/>
+      <c r="C22" s="40"/>
       <c r="D22" s="6">
         <v>1.25</v>
       </c>
@@ -1405,9 +1405,9 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="31"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
+      <c r="A23" s="46"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
       <c r="D23" s="6">
         <v>1.5</v>
       </c>
@@ -1426,9 +1426,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="31"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
+      <c r="A24" s="46"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
       <c r="D24" s="6">
         <v>1.75</v>
       </c>
@@ -1448,9 +1448,9 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="31"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
+      <c r="A25" s="46"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
       <c r="D25" s="6">
         <v>2</v>
       </c>
@@ -1470,11 +1470,11 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="31"/>
-      <c r="B26" s="34">
+      <c r="A26" s="46"/>
+      <c r="B26" s="40">
         <v>0.5</v>
       </c>
-      <c r="C26" s="34"/>
+      <c r="C26" s="40"/>
       <c r="D26" s="6">
         <v>1.25</v>
       </c>
@@ -1494,9 +1494,9 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="31"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
+      <c r="A27" s="46"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
       <c r="D27" s="6">
         <v>1.5</v>
       </c>
@@ -1516,9 +1516,9 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="31"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
+      <c r="A28" s="46"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
       <c r="D28" s="6">
         <v>1.75</v>
       </c>
@@ -1538,9 +1538,9 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="31"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
+      <c r="A29" s="46"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
       <c r="D29" s="6">
         <v>2</v>
       </c>
@@ -1560,11 +1560,11 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="31"/>
-      <c r="B30" s="34">
+      <c r="A30" s="46"/>
+      <c r="B30" s="40">
         <v>0.25</v>
       </c>
-      <c r="C30" s="34"/>
+      <c r="C30" s="40"/>
       <c r="D30" s="6">
         <v>1.25</v>
       </c>
@@ -1584,9 +1584,9 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="31"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
+      <c r="A31" s="46"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
       <c r="D31" s="6">
         <v>1.5</v>
       </c>
@@ -1606,9 +1606,9 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="31"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
+      <c r="A32" s="46"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
       <c r="D32" s="6">
         <v>1.75</v>
       </c>
@@ -1628,9 +1628,9 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="32"/>
-      <c r="B33" s="35"/>
-      <c r="C33" s="35"/>
+      <c r="A33" s="47"/>
+      <c r="B33" s="41"/>
+      <c r="C33" s="41"/>
       <c r="D33" s="8">
         <v>2</v>
       </c>
@@ -1650,13 +1650,13 @@
       <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="44" t="s">
+      <c r="A34" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="47">
+      <c r="B34" s="39">
         <v>0.1</v>
       </c>
-      <c r="C34" s="47">
+      <c r="C34" s="39">
         <v>1</v>
       </c>
       <c r="D34" s="4">
@@ -1678,9 +1678,9 @@
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="45"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
+      <c r="A35" s="37"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
       <c r="D35" s="6">
         <v>1.5</v>
       </c>
@@ -1700,9 +1700,9 @@
       <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="45"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
+      <c r="A36" s="37"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
       <c r="D36" s="6">
         <v>1.75</v>
       </c>
@@ -1722,9 +1722,9 @@
       <c r="I36" s="10"/>
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="46"/>
-      <c r="B37" s="35"/>
-      <c r="C37" s="35"/>
+      <c r="A37" s="38"/>
+      <c r="B37" s="41"/>
+      <c r="C37" s="41"/>
       <c r="D37" s="8">
         <v>2</v>
       </c>
@@ -1747,11 +1747,11 @@
       <c r="A38" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="48" t="s">
+      <c r="B38" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="49"/>
-      <c r="D38" s="50"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="44"/>
       <c r="E38" s="8">
         <v>43.123899999999999</v>
       </c>
@@ -1771,10 +1771,10 @@
       <c r="A39" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="39" t="s">
+      <c r="B39" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C39" s="40"/>
+      <c r="C39" s="32"/>
       <c r="D39" s="20" t="s">
         <v>12</v>
       </c>
@@ -1799,11 +1799,11 @@
       <c r="A40" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B40" s="41" t="s">
+      <c r="B40" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="42"/>
-      <c r="D40" s="43"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="35"/>
       <c r="E40" s="22">
         <v>43.224200000000003</v>
       </c>
@@ -1820,12 +1820,12 @@
       <c r="I40" s="10"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="38" t="s">
+      <c r="A41" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="38"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
       <c r="E41" s="5">
         <v>42.909700000000001</v>
       </c>
@@ -1852,13 +1852,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="B38:D38"/>
     <mergeCell ref="A2:A33"/>
     <mergeCell ref="B2:B17"/>
     <mergeCell ref="C2:C5"/>
@@ -1869,6 +1862,13 @@
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B30:B33"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="B38:D38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1918,10 +1918,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="51">
+      <c r="B2" s="52">
         <v>4</v>
       </c>
       <c r="C2" s="25">
@@ -1942,8 +1942,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="52"/>
-      <c r="B3" s="52"/>
+      <c r="A3" s="53"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="24">
         <v>1.5</v>
       </c>
@@ -1963,8 +1963,8 @@
       <c r="I3" s="28"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="52"/>
-      <c r="B4" s="52"/>
+      <c r="A4" s="53"/>
+      <c r="B4" s="53"/>
       <c r="C4" s="24">
         <v>1.75</v>
       </c>
@@ -1983,8 +1983,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
-      <c r="B5" s="53"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="54"/>
       <c r="C5" s="24">
         <v>2</v>
       </c>
@@ -2003,8 +2003,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="52"/>
-      <c r="B6" s="54">
+      <c r="A6" s="53"/>
+      <c r="B6" s="55">
         <v>5</v>
       </c>
       <c r="C6" s="25">
@@ -2025,8 +2025,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="52"/>
-      <c r="B7" s="52"/>
+      <c r="A7" s="53"/>
+      <c r="B7" s="53"/>
       <c r="C7" s="24">
         <v>1.5</v>
       </c>
@@ -2045,8 +2045,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="52"/>
-      <c r="B8" s="52"/>
+      <c r="A8" s="53"/>
+      <c r="B8" s="53"/>
       <c r="C8" s="24">
         <v>1.75</v>
       </c>
@@ -2065,8 +2065,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="52"/>
-      <c r="B9" s="53"/>
+      <c r="A9" s="53"/>
+      <c r="B9" s="54"/>
       <c r="C9" s="24">
         <v>2</v>
       </c>
@@ -2085,8 +2085,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="52"/>
-      <c r="B10" s="54">
+      <c r="A10" s="53"/>
+      <c r="B10" s="55">
         <v>6</v>
       </c>
       <c r="C10" s="25">
@@ -2107,8 +2107,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="52"/>
-      <c r="B11" s="52"/>
+      <c r="A11" s="53"/>
+      <c r="B11" s="53"/>
       <c r="C11" s="24">
         <v>1.5</v>
       </c>
@@ -2127,8 +2127,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="52"/>
-      <c r="B12" s="52"/>
+      <c r="A12" s="53"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="24">
         <v>1.75</v>
       </c>
@@ -2147,8 +2147,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="52"/>
-      <c r="B13" s="53"/>
+      <c r="A13" s="53"/>
+      <c r="B13" s="54"/>
       <c r="C13" s="24">
         <v>2</v>
       </c>
@@ -2167,8 +2167,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="52"/>
-      <c r="B14" s="54">
+      <c r="A14" s="53"/>
+      <c r="B14" s="55">
         <v>7</v>
       </c>
       <c r="C14" s="25">
@@ -2189,8 +2189,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="52"/>
-      <c r="B15" s="52"/>
+      <c r="A15" s="53"/>
+      <c r="B15" s="53"/>
       <c r="C15" s="24">
         <v>1.5</v>
       </c>
@@ -2209,8 +2209,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="52"/>
-      <c r="B16" s="52"/>
+      <c r="A16" s="53"/>
+      <c r="B16" s="53"/>
       <c r="C16" s="24">
         <v>1.75</v>
       </c>
@@ -2229,8 +2229,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="53"/>
-      <c r="B17" s="53"/>
+      <c r="A17" s="54"/>
+      <c r="B17" s="54"/>
       <c r="C17" s="24">
         <v>2</v>
       </c>
@@ -2249,10 +2249,10 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="55">
+      <c r="B18" s="51">
         <v>4</v>
       </c>
       <c r="C18" s="25">
@@ -2273,8 +2273,8 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="37"/>
-      <c r="B19" s="55"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="51"/>
       <c r="C19" s="24">
         <v>1.5</v>
       </c>
@@ -2293,8 +2293,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="37"/>
-      <c r="B20" s="55"/>
+      <c r="A20" s="50"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="24">
         <v>1.75</v>
       </c>
@@ -2313,8 +2313,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="37"/>
-      <c r="B21" s="55"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="51"/>
       <c r="C21" s="24">
         <v>2</v>
       </c>
@@ -2333,8 +2333,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="37"/>
-      <c r="B22" s="55">
+      <c r="A22" s="50"/>
+      <c r="B22" s="51">
         <v>5</v>
       </c>
       <c r="C22" s="25">
@@ -2355,8 +2355,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="37"/>
-      <c r="B23" s="55"/>
+      <c r="A23" s="50"/>
+      <c r="B23" s="51"/>
       <c r="C23" s="24">
         <v>1.5</v>
       </c>
@@ -2375,8 +2375,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="37"/>
-      <c r="B24" s="55"/>
+      <c r="A24" s="50"/>
+      <c r="B24" s="51"/>
       <c r="C24" s="24">
         <v>1.75</v>
       </c>
@@ -2398,8 +2398,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="37"/>
-      <c r="B25" s="55"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="51"/>
       <c r="C25" s="24">
         <v>2</v>
       </c>
@@ -2418,8 +2418,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="37"/>
-      <c r="B26" s="55">
+      <c r="A26" s="50"/>
+      <c r="B26" s="51">
         <v>6</v>
       </c>
       <c r="C26" s="25">
@@ -2440,8 +2440,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="37"/>
-      <c r="B27" s="55"/>
+      <c r="A27" s="50"/>
+      <c r="B27" s="51"/>
       <c r="C27" s="24">
         <v>1.5</v>
       </c>
@@ -2460,8 +2460,8 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="37"/>
-      <c r="B28" s="55"/>
+      <c r="A28" s="50"/>
+      <c r="B28" s="51"/>
       <c r="C28" s="24">
         <v>1.75</v>
       </c>
@@ -2480,8 +2480,8 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="37"/>
-      <c r="B29" s="55"/>
+      <c r="A29" s="50"/>
+      <c r="B29" s="51"/>
       <c r="C29" s="24">
         <v>2</v>
       </c>
@@ -2500,8 +2500,8 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="37"/>
-      <c r="B30" s="55">
+      <c r="A30" s="50"/>
+      <c r="B30" s="51">
         <v>7</v>
       </c>
       <c r="C30" s="25">
@@ -2522,8 +2522,8 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="37"/>
-      <c r="B31" s="55"/>
+      <c r="A31" s="50"/>
+      <c r="B31" s="51"/>
       <c r="C31" s="24">
         <v>1.5</v>
       </c>
@@ -2542,8 +2542,8 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="37"/>
-      <c r="B32" s="55"/>
+      <c r="A32" s="50"/>
+      <c r="B32" s="51"/>
       <c r="C32" s="24">
         <v>1.75</v>
       </c>
@@ -2562,8 +2562,8 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="33"/>
-      <c r="B33" s="55"/>
+      <c r="A33" s="48"/>
+      <c r="B33" s="51"/>
       <c r="C33" s="24">
         <v>2</v>
       </c>
@@ -2583,16 +2583,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="A18:A33"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2642,10 +2642,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="51">
+      <c r="B2" s="52">
         <v>0.2</v>
       </c>
       <c r="C2" s="25">
@@ -2666,8 +2666,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="52"/>
-      <c r="B3" s="52"/>
+      <c r="A3" s="53"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="24">
         <v>1.5</v>
       </c>
@@ -2686,8 +2686,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="52"/>
-      <c r="B4" s="52"/>
+      <c r="A4" s="53"/>
+      <c r="B4" s="53"/>
       <c r="C4" s="24">
         <v>1.75</v>
       </c>
@@ -2706,8 +2706,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
-      <c r="B5" s="53"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="54"/>
       <c r="C5" s="24">
         <v>2</v>
       </c>
@@ -2726,8 +2726,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="52"/>
-      <c r="B6" s="54">
+      <c r="A6" s="53"/>
+      <c r="B6" s="55">
         <v>0.4</v>
       </c>
       <c r="C6" s="25">
@@ -2748,8 +2748,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="52"/>
-      <c r="B7" s="52"/>
+      <c r="A7" s="53"/>
+      <c r="B7" s="53"/>
       <c r="C7" s="24">
         <v>1.5</v>
       </c>
@@ -2768,8 +2768,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="52"/>
-      <c r="B8" s="52"/>
+      <c r="A8" s="53"/>
+      <c r="B8" s="53"/>
       <c r="C8" s="24">
         <v>1.75</v>
       </c>
@@ -2788,8 +2788,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="52"/>
-      <c r="B9" s="53"/>
+      <c r="A9" s="53"/>
+      <c r="B9" s="54"/>
       <c r="C9" s="24">
         <v>2</v>
       </c>
@@ -2808,8 +2808,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="52"/>
-      <c r="B10" s="54">
+      <c r="A10" s="53"/>
+      <c r="B10" s="55">
         <v>0.6</v>
       </c>
       <c r="C10" s="25">
@@ -2830,8 +2830,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="52"/>
-      <c r="B11" s="52"/>
+      <c r="A11" s="53"/>
+      <c r="B11" s="53"/>
       <c r="C11" s="24">
         <v>1.5</v>
       </c>
@@ -2850,8 +2850,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="52"/>
-      <c r="B12" s="52"/>
+      <c r="A12" s="53"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="24">
         <v>1.75</v>
       </c>
@@ -2870,8 +2870,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="52"/>
-      <c r="B13" s="53"/>
+      <c r="A13" s="53"/>
+      <c r="B13" s="54"/>
       <c r="C13" s="24">
         <v>2</v>
       </c>
@@ -2890,8 +2890,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="52"/>
-      <c r="B14" s="55">
+      <c r="A14" s="53"/>
+      <c r="B14" s="51">
         <v>0.8</v>
       </c>
       <c r="C14" s="25">
@@ -2912,8 +2912,8 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="52"/>
-      <c r="B15" s="55"/>
+      <c r="A15" s="53"/>
+      <c r="B15" s="51"/>
       <c r="C15" s="24">
         <v>1.5</v>
       </c>
@@ -2932,8 +2932,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="52"/>
-      <c r="B16" s="55"/>
+      <c r="A16" s="53"/>
+      <c r="B16" s="51"/>
       <c r="C16" s="24">
         <v>1.75</v>
       </c>
@@ -2952,8 +2952,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="53"/>
-      <c r="B17" s="55"/>
+      <c r="A17" s="54"/>
+      <c r="B17" s="51"/>
       <c r="C17" s="24">
         <v>2</v>
       </c>
@@ -2972,10 +2972,10 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="52">
+      <c r="B18" s="53">
         <v>0.2</v>
       </c>
       <c r="C18" s="25">
@@ -2996,8 +2996,8 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="37"/>
-      <c r="B19" s="52"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="53"/>
       <c r="C19" s="24">
         <v>1.5</v>
       </c>
@@ -3016,8 +3016,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="37"/>
-      <c r="B20" s="52"/>
+      <c r="A20" s="50"/>
+      <c r="B20" s="53"/>
       <c r="C20" s="24">
         <v>1.75</v>
       </c>
@@ -3036,8 +3036,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="37"/>
-      <c r="B21" s="53"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="54"/>
       <c r="C21" s="24">
         <v>2</v>
       </c>
@@ -3056,8 +3056,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="37"/>
-      <c r="B22" s="54">
+      <c r="A22" s="50"/>
+      <c r="B22" s="55">
         <v>0.4</v>
       </c>
       <c r="C22" s="25">
@@ -3081,8 +3081,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="37"/>
-      <c r="B23" s="52"/>
+      <c r="A23" s="50"/>
+      <c r="B23" s="53"/>
       <c r="C23" s="24">
         <v>1.5</v>
       </c>
@@ -3101,8 +3101,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="37"/>
-      <c r="B24" s="52"/>
+      <c r="A24" s="50"/>
+      <c r="B24" s="53"/>
       <c r="C24" s="24">
         <v>1.75</v>
       </c>
@@ -3121,8 +3121,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="37"/>
-      <c r="B25" s="53"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="54"/>
       <c r="C25" s="24">
         <v>2</v>
       </c>
@@ -3141,8 +3141,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="37"/>
-      <c r="B26" s="54">
+      <c r="A26" s="50"/>
+      <c r="B26" s="55">
         <v>0.6</v>
       </c>
       <c r="C26" s="25">
@@ -3163,8 +3163,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="37"/>
-      <c r="B27" s="52"/>
+      <c r="A27" s="50"/>
+      <c r="B27" s="53"/>
       <c r="C27" s="24">
         <v>1.5</v>
       </c>
@@ -3183,8 +3183,8 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="37"/>
-      <c r="B28" s="52"/>
+      <c r="A28" s="50"/>
+      <c r="B28" s="53"/>
       <c r="C28" s="24">
         <v>1.75</v>
       </c>
@@ -3203,8 +3203,8 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="37"/>
-      <c r="B29" s="53"/>
+      <c r="A29" s="50"/>
+      <c r="B29" s="54"/>
       <c r="C29" s="24">
         <v>2</v>
       </c>
@@ -3223,8 +3223,8 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="37"/>
-      <c r="B30" s="54">
+      <c r="A30" s="50"/>
+      <c r="B30" s="55">
         <v>0.8</v>
       </c>
       <c r="C30" s="25">
@@ -3245,8 +3245,8 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="37"/>
-      <c r="B31" s="52"/>
+      <c r="A31" s="50"/>
+      <c r="B31" s="53"/>
       <c r="C31" s="24">
         <v>1.5</v>
       </c>
@@ -3265,8 +3265,8 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="37"/>
-      <c r="B32" s="52"/>
+      <c r="A32" s="50"/>
+      <c r="B32" s="53"/>
       <c r="C32" s="24">
         <v>1.75</v>
       </c>
@@ -3285,8 +3285,8 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="33"/>
-      <c r="B33" s="53"/>
+      <c r="A33" s="48"/>
+      <c r="B33" s="54"/>
       <c r="C33" s="24">
         <v>2</v>
       </c>
@@ -3307,16 +3307,16 @@
     <row r="42" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="A18:A33"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3327,7 +3327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EC75104-98F5-44A7-8EFA-4A397559D5FA}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
@@ -3366,10 +3366,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="51">
+      <c r="B2" s="52">
         <v>0</v>
       </c>
       <c r="C2" s="25">
@@ -3390,8 +3390,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="52"/>
-      <c r="B3" s="52"/>
+      <c r="A3" s="53"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="24">
         <v>1.5</v>
       </c>
@@ -3410,8 +3410,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="52"/>
-      <c r="B4" s="52"/>
+      <c r="A4" s="53"/>
+      <c r="B4" s="53"/>
       <c r="C4" s="24">
         <v>1.75</v>
       </c>
@@ -3424,8 +3424,8 @@
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
-      <c r="B5" s="53"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="54"/>
       <c r="C5" s="24">
         <v>2</v>
       </c>
@@ -3438,8 +3438,8 @@
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="52"/>
-      <c r="B6" s="54">
+      <c r="A6" s="53"/>
+      <c r="B6" s="55">
         <v>1</v>
       </c>
       <c r="C6" s="25">
@@ -3454,8 +3454,8 @@
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="52"/>
-      <c r="B7" s="52"/>
+      <c r="A7" s="53"/>
+      <c r="B7" s="53"/>
       <c r="C7" s="24">
         <v>1.5</v>
       </c>
@@ -3474,8 +3474,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="52"/>
-      <c r="B8" s="52"/>
+      <c r="A8" s="53"/>
+      <c r="B8" s="53"/>
       <c r="C8" s="24">
         <v>1.75</v>
       </c>
@@ -3494,8 +3494,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="52"/>
-      <c r="B9" s="53"/>
+      <c r="A9" s="53"/>
+      <c r="B9" s="54"/>
       <c r="C9" s="24">
         <v>2</v>
       </c>
@@ -3514,8 +3514,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="52"/>
-      <c r="B10" s="54">
+      <c r="A10" s="53"/>
+      <c r="B10" s="55">
         <v>2</v>
       </c>
       <c r="C10" s="25">
@@ -3536,8 +3536,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="52"/>
-      <c r="B11" s="52"/>
+      <c r="A11" s="53"/>
+      <c r="B11" s="53"/>
       <c r="C11" s="24">
         <v>1.5</v>
       </c>
@@ -3556,8 +3556,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="52"/>
-      <c r="B12" s="52"/>
+      <c r="A12" s="53"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="24">
         <v>1.75</v>
       </c>
@@ -3576,8 +3576,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="52"/>
-      <c r="B13" s="53"/>
+      <c r="A13" s="53"/>
+      <c r="B13" s="54"/>
       <c r="C13" s="24">
         <v>2</v>
       </c>
@@ -3596,8 +3596,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="52"/>
-      <c r="B14" s="54">
+      <c r="A14" s="53"/>
+      <c r="B14" s="55">
         <v>3</v>
       </c>
       <c r="C14" s="25">
@@ -3618,8 +3618,8 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="52"/>
-      <c r="B15" s="52"/>
+      <c r="A15" s="53"/>
+      <c r="B15" s="53"/>
       <c r="C15" s="24">
         <v>1.5</v>
       </c>
@@ -3638,8 +3638,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="52"/>
-      <c r="B16" s="52"/>
+      <c r="A16" s="53"/>
+      <c r="B16" s="53"/>
       <c r="C16" s="24">
         <v>1.75</v>
       </c>
@@ -3658,8 +3658,8 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="53"/>
-      <c r="B17" s="53"/>
+      <c r="A17" s="54"/>
+      <c r="B17" s="54"/>
       <c r="C17" s="24">
         <v>2</v>
       </c>
@@ -3678,10 +3678,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="55">
+      <c r="B18" s="51">
         <v>0</v>
       </c>
       <c r="C18" s="25">
@@ -3702,8 +3702,8 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="37"/>
-      <c r="B19" s="55"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="51"/>
       <c r="C19" s="24">
         <v>1.5</v>
       </c>
@@ -3722,8 +3722,8 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="37"/>
-      <c r="B20" s="55"/>
+      <c r="A20" s="50"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="24">
         <v>1.75</v>
       </c>
@@ -3742,8 +3742,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="37"/>
-      <c r="B21" s="55"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="51"/>
       <c r="C21" s="24">
         <v>2</v>
       </c>
@@ -3762,8 +3762,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="37"/>
-      <c r="B22" s="55">
+      <c r="A22" s="50"/>
+      <c r="B22" s="51">
         <v>1</v>
       </c>
       <c r="C22" s="25">
@@ -3784,8 +3784,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="37"/>
-      <c r="B23" s="55"/>
+      <c r="A23" s="50"/>
+      <c r="B23" s="51"/>
       <c r="C23" s="24">
         <v>1.5</v>
       </c>
@@ -3804,8 +3804,8 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="37"/>
-      <c r="B24" s="55"/>
+      <c r="A24" s="50"/>
+      <c r="B24" s="51"/>
       <c r="C24" s="24">
         <v>1.75</v>
       </c>
@@ -3824,8 +3824,8 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="37"/>
-      <c r="B25" s="55"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="51"/>
       <c r="C25" s="24">
         <v>2</v>
       </c>
@@ -3844,8 +3844,8 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="37"/>
-      <c r="B26" s="55">
+      <c r="A26" s="50"/>
+      <c r="B26" s="51">
         <v>2</v>
       </c>
       <c r="C26" s="25">
@@ -3866,8 +3866,8 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="37"/>
-      <c r="B27" s="55"/>
+      <c r="A27" s="50"/>
+      <c r="B27" s="51"/>
       <c r="C27" s="24">
         <v>1.5</v>
       </c>
@@ -3886,8 +3886,8 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="37"/>
-      <c r="B28" s="55"/>
+      <c r="A28" s="50"/>
+      <c r="B28" s="51"/>
       <c r="C28" s="24">
         <v>1.75</v>
       </c>
@@ -3906,8 +3906,8 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="37"/>
-      <c r="B29" s="55"/>
+      <c r="A29" s="50"/>
+      <c r="B29" s="51"/>
       <c r="C29" s="24">
         <v>2</v>
       </c>
@@ -3926,8 +3926,8 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="37"/>
-      <c r="B30" s="55">
+      <c r="A30" s="50"/>
+      <c r="B30" s="51">
         <v>3</v>
       </c>
       <c r="C30" s="25">
@@ -3948,8 +3948,8 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="37"/>
-      <c r="B31" s="55"/>
+      <c r="A31" s="50"/>
+      <c r="B31" s="51"/>
       <c r="C31" s="24">
         <v>1.5</v>
       </c>
@@ -3968,8 +3968,8 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="37"/>
-      <c r="B32" s="55"/>
+      <c r="A32" s="50"/>
+      <c r="B32" s="51"/>
       <c r="C32" s="24">
         <v>1.75</v>
       </c>
@@ -3988,8 +3988,8 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="33"/>
-      <c r="B33" s="55"/>
+      <c r="A33" s="48"/>
+      <c r="B33" s="51"/>
       <c r="C33" s="24">
         <v>2</v>
       </c>
@@ -4009,16 +4009,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="A18:A33"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -4029,8 +4029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90522F64-6716-4420-BD73-4405BBA33BC6}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4064,115 +4064,163 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="51">
+      <c r="A2" s="52">
         <v>4</v>
       </c>
       <c r="B2" s="25">
         <v>1.25</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="12"/>
+      <c r="C2" s="4">
+        <v>42.905799999999999</v>
+      </c>
+      <c r="D2" s="12">
+        <v>26138.2539</v>
+      </c>
       <c r="E2" s="5">
         <f>D2/3600</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="5"/>
+        <v>7.2606260833333334</v>
+      </c>
+      <c r="F2" s="5">
+        <v>258.44920000000002</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="52"/>
+      <c r="A3" s="53"/>
       <c r="B3" s="24">
         <v>1.5</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="13"/>
+      <c r="C3" s="6">
+        <v>42.916499999999999</v>
+      </c>
+      <c r="D3" s="13">
+        <v>17367.591799999998</v>
+      </c>
       <c r="E3" s="5">
         <f t="shared" ref="E3:E17" si="0">D3/3600</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="7"/>
+        <v>4.8243310555555547</v>
+      </c>
+      <c r="F3" s="7">
+        <v>103.4242</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="52"/>
+      <c r="A4" s="53"/>
       <c r="B4" s="24">
         <v>1.75</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="13"/>
+      <c r="C4" s="6">
+        <v>43.137700000000002</v>
+      </c>
+      <c r="D4" s="13">
+        <v>21418.279299999998</v>
+      </c>
       <c r="E4" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F4" s="7"/>
+        <v>5.9495220277777774</v>
+      </c>
+      <c r="F4" s="7">
+        <v>232.65119999999999</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="53"/>
+      <c r="A5" s="54"/>
       <c r="B5" s="24">
         <v>2</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="13"/>
+      <c r="C5" s="6">
+        <v>43.3065</v>
+      </c>
+      <c r="D5" s="13">
+        <v>27538.761200000001</v>
+      </c>
       <c r="E5" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F5" s="7"/>
+        <v>7.6496558888888888</v>
+      </c>
+      <c r="F5" s="5">
+        <v>258.44920000000002</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="54">
+      <c r="A6" s="55">
         <v>5</v>
       </c>
       <c r="B6" s="25">
         <v>1.25</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="13"/>
+      <c r="C6" s="6">
+        <v>42.793900000000001</v>
+      </c>
+      <c r="D6" s="13">
+        <v>16372.566000000001</v>
+      </c>
       <c r="E6" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="7"/>
+        <v>4.5479349999999998</v>
+      </c>
+      <c r="F6" s="7">
+        <v>206.76740000000001</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="52"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="24">
         <v>1.5</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="13"/>
+      <c r="C7" s="6">
+        <v>43.243200000000002</v>
+      </c>
+      <c r="D7" s="13">
+        <v>27641.671300000002</v>
+      </c>
       <c r="E7" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="7"/>
+        <v>7.6782420277777783</v>
+      </c>
+      <c r="F7" s="5">
+        <v>258.44920000000002</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="52"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="24">
         <v>1.75</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="13"/>
+      <c r="C8" s="6">
+        <v>43.277099999999997</v>
+      </c>
+      <c r="D8" s="13">
+        <v>27532.234899999999</v>
+      </c>
       <c r="E8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="7"/>
+        <v>7.6478430277777774</v>
+      </c>
+      <c r="F8" s="5">
+        <v>258.44920000000002</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="53"/>
+      <c r="A9" s="54"/>
       <c r="B9" s="24">
         <v>2</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="13"/>
+      <c r="C9" s="6">
+        <v>42.643099999999997</v>
+      </c>
+      <c r="D9" s="13">
+        <v>17365.373299999999</v>
+      </c>
       <c r="E9" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="7"/>
+        <v>4.8237148055555554</v>
+      </c>
+      <c r="F9" s="7">
+        <v>232.65119999999999</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="54">
+      <c r="A10" s="55">
         <v>6</v>
       </c>
       <c r="B10" s="25">
@@ -4187,20 +4235,26 @@
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="52"/>
+      <c r="A11" s="53"/>
       <c r="B11" s="24">
         <v>1.5</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="13"/>
+      <c r="C11" s="6">
+        <v>42.703400000000002</v>
+      </c>
+      <c r="D11" s="13">
+        <v>13376.0388</v>
+      </c>
       <c r="E11" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="7"/>
+        <v>3.7155663333333333</v>
+      </c>
+      <c r="F11" s="7">
+        <v>155.0676</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="52"/>
+      <c r="A12" s="53"/>
       <c r="B12" s="24">
         <v>1.75</v>
       </c>
@@ -4213,7 +4267,7 @@
       <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="53"/>
+      <c r="A13" s="54"/>
       <c r="B13" s="24">
         <v>2</v>
       </c>
@@ -4226,7 +4280,7 @@
       <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="54">
+      <c r="A14" s="55">
         <v>7</v>
       </c>
       <c r="B14" s="25">
@@ -4241,33 +4295,45 @@
       <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="52"/>
+      <c r="A15" s="53"/>
       <c r="B15" s="24">
         <v>1.5</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="13"/>
+      <c r="C15" s="6">
+        <v>43.299399999999999</v>
+      </c>
+      <c r="D15" s="13">
+        <v>24647.067299999999</v>
+      </c>
       <c r="E15" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="7"/>
+        <v>6.8464075833333329</v>
+      </c>
+      <c r="F15" s="7">
+        <v>310.13979999999998</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="52"/>
+      <c r="A16" s="53"/>
       <c r="B16" s="24">
         <v>1.75</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="13"/>
+      <c r="C16" s="6">
+        <v>43.002000000000002</v>
+      </c>
+      <c r="D16" s="13">
+        <v>17406.909199999998</v>
+      </c>
       <c r="E16" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="7"/>
+        <v>4.835252555555555</v>
+      </c>
+      <c r="F16" s="7">
+        <v>206.76740000000001</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="53"/>
+      <c r="A17" s="54"/>
       <c r="B17" s="24">
         <v>2</v>
       </c>
@@ -4432,7 +4498,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E17"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4466,7 +4532,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="51">
+      <c r="A2" s="52">
         <v>0.2</v>
       </c>
       <c r="B2" s="25">
@@ -4481,7 +4547,7 @@
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="52"/>
+      <c r="A3" s="53"/>
       <c r="B3" s="24">
         <v>1.5</v>
       </c>
@@ -4494,7 +4560,7 @@
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="52"/>
+      <c r="A4" s="53"/>
       <c r="B4" s="24">
         <v>1.75</v>
       </c>
@@ -4507,7 +4573,7 @@
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="53"/>
+      <c r="A5" s="54"/>
       <c r="B5" s="24">
         <v>2</v>
       </c>
@@ -4520,7 +4586,7 @@
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="54">
+      <c r="A6" s="55">
         <v>0.4</v>
       </c>
       <c r="B6" s="25">
@@ -4535,7 +4601,7 @@
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="52"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="24">
         <v>1.5</v>
       </c>
@@ -4548,7 +4614,7 @@
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="52"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="24">
         <v>1.75</v>
       </c>
@@ -4561,7 +4627,7 @@
       <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="53"/>
+      <c r="A9" s="54"/>
       <c r="B9" s="24">
         <v>2</v>
       </c>
@@ -4574,7 +4640,7 @@
       <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="54">
+      <c r="A10" s="55">
         <v>0.6</v>
       </c>
       <c r="B10" s="25">
@@ -4589,7 +4655,7 @@
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="52"/>
+      <c r="A11" s="53"/>
       <c r="B11" s="24">
         <v>1.5</v>
       </c>
@@ -4602,7 +4668,7 @@
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="52"/>
+      <c r="A12" s="53"/>
       <c r="B12" s="24">
         <v>1.75</v>
       </c>
@@ -4615,7 +4681,7 @@
       <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="53"/>
+      <c r="A13" s="54"/>
       <c r="B13" s="24">
         <v>2</v>
       </c>
@@ -4628,7 +4694,7 @@
       <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="55">
+      <c r="A14" s="51">
         <v>0.8</v>
       </c>
       <c r="B14" s="25">
@@ -4643,7 +4709,7 @@
       <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="55"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="24">
         <v>1.5</v>
       </c>
@@ -4656,7 +4722,7 @@
       <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="55"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="24">
         <v>1.75</v>
       </c>
@@ -4669,7 +4735,7 @@
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="55"/>
+      <c r="A17" s="51"/>
       <c r="B17" s="24">
         <v>2</v>
       </c>
@@ -4851,7 +4917,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4885,7 +4951,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="51">
+      <c r="A2" s="52">
         <v>0</v>
       </c>
       <c r="B2" s="25">
@@ -4900,7 +4966,7 @@
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="52"/>
+      <c r="A3" s="53"/>
       <c r="B3" s="24">
         <v>1.5</v>
       </c>
@@ -4913,7 +4979,7 @@
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="52"/>
+      <c r="A4" s="53"/>
       <c r="B4" s="24">
         <v>1.75</v>
       </c>
@@ -4926,7 +4992,7 @@
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="53"/>
+      <c r="A5" s="54"/>
       <c r="B5" s="24">
         <v>2</v>
       </c>
@@ -4939,7 +5005,7 @@
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="54">
+      <c r="A6" s="55">
         <v>1</v>
       </c>
       <c r="B6" s="25">
@@ -4954,7 +5020,7 @@
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="52"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="24">
         <v>1.5</v>
       </c>
@@ -4967,7 +5033,7 @@
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="52"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="24">
         <v>1.75</v>
       </c>
@@ -4980,7 +5046,7 @@
       <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="53"/>
+      <c r="A9" s="54"/>
       <c r="B9" s="24">
         <v>2</v>
       </c>
@@ -4993,7 +5059,7 @@
       <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="54">
+      <c r="A10" s="55">
         <v>2</v>
       </c>
       <c r="B10" s="25">
@@ -5008,7 +5074,7 @@
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="52"/>
+      <c r="A11" s="53"/>
       <c r="B11" s="24">
         <v>1.5</v>
       </c>
@@ -5021,7 +5087,7 @@
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="52"/>
+      <c r="A12" s="53"/>
       <c r="B12" s="24">
         <v>1.75</v>
       </c>
@@ -5034,7 +5100,7 @@
       <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="53"/>
+      <c r="A13" s="54"/>
       <c r="B13" s="24">
         <v>2</v>
       </c>
@@ -5047,7 +5113,7 @@
       <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="54">
+      <c r="A14" s="55">
         <v>3</v>
       </c>
       <c r="B14" s="25">
@@ -5062,7 +5128,7 @@
       <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="52"/>
+      <c r="A15" s="53"/>
       <c r="B15" s="24">
         <v>1.5</v>
       </c>
@@ -5075,7 +5141,7 @@
       <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="52"/>
+      <c r="A16" s="53"/>
       <c r="B16" s="24">
         <v>1.75</v>
       </c>
@@ -5088,7 +5154,7 @@
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="53"/>
+      <c r="A17" s="54"/>
       <c r="B17" s="24">
         <v>2</v>
       </c>
@@ -5273,11 +5339,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5510,27 +5577,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5555,9 +5612,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>